<commit_message>
Dec 9 data and improved graphs
</commit_message>
<xml_diff>
--- a/data/CasesByAge.xlsx
+++ b/data/CasesByAge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV filesPROB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E2033E-6F52-474E-B564-82D4F8A627A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CFF6B9-03CA-4E4A-B21E-1CAFC1645442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D024909B-A8AA-47FC-869B-1DA071808E97}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D024909B-A8AA-47FC-869B-1DA071808E97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -420,21 +423,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE62140-7A80-49E1-B591-358B146BFD65}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="10" max="10" width="41.1796875" customWidth="1"/>
-    <col min="11" max="11" width="21.453125" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="41.21875" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +475,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44137</v>
       </c>
@@ -510,7 +513,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44139</v>
       </c>
@@ -548,7 +551,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44146</v>
       </c>
@@ -586,7 +589,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44153</v>
       </c>
@@ -624,7 +627,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44160</v>
       </c>
@@ -662,7 +665,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44167</v>
       </c>
@@ -698,6 +701,44 @@
       </c>
       <c r="L7">
         <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44174</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8201</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9746</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8174</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6835</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7141</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4683</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2317</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1676</v>
+      </c>
+      <c r="J8" s="1">
+        <v>69</v>
+      </c>
+      <c r="K8" s="1">
+        <v>82</v>
+      </c>
+      <c r="L8" s="1">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big update for 02Jan
</commit_message>
<xml_diff>
--- a/data/CasesByAge.xlsx
+++ b/data/CasesByAge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\COVID-19 Data Visualization\COVID19 - Files\Power BI resources\CSV filesPROB4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37194E5E-1707-42E0-ADA4-AAA5C644246F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476BE2A8-95D7-40CE-A822-DBE86B9B98C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D024909B-A8AA-47FC-869B-1DA071808E97}"/>
   </bookViews>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE62140-7A80-49E1-B591-358B146BFD65}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,6 +817,44 @@
         <v>63.2</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>44195</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9814</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9907</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8822</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7895</v>
+      </c>
+      <c r="F11" s="1">
+        <v>8695</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6156</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3121</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2441</v>
+      </c>
+      <c r="J11" s="1">
+        <v>73</v>
+      </c>
+      <c r="K11" s="1">
+        <v>81</v>
+      </c>
+      <c r="L11">
+        <v>58.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>